<commit_message>
refactored code for Sabra and Shatila massacre
</commit_message>
<xml_diff>
--- a/POST-THESIS/1982/entity_creation/datasets_updated/Sabra_and_Shatila_massacre/locations_ar.xlsx
+++ b/POST-THESIS/1982/entity_creation/datasets_updated/Sabra_and_Shatila_massacre/locations_ar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,41 +470,41 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">علم الدولة (مترجمه),لبنان </t>
+          <t>-</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">بلد </t>
+          <t>-</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">بكفيا </t>
+          <t xml:space="preserve">العراق </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>لبنان (مترجمه)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">بلد </t>
+          <t>-</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">بشري (لبنان) </t>
+          <t xml:space="preserve">لبنان </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>لبنان (مترجمه)</t>
+          <t>الاستخبارات والمراقبة والرصد (مترجمه)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -514,14 +514,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">الدامور </t>
+          <t xml:space="preserve">نهاريا </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">علم الدولة (مترجمه),لبنان </t>
+          <t xml:space="preserve">لبنان </t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -531,41 +531,41 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">إهدن </t>
+          <t>صبرة (مترجمه)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve">الانتداب البريطاني على فلسطين </t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve">علم الوجود الجغرافي السياسي </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">إسرائيل </t>
+          <t xml:space="preserve">صلحا </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">لبنان ,علم (راية) </t>
+          <t>-</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">بلد </t>
+          <t>-</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">قضاء كسروان </t>
+          <t xml:space="preserve">سنغافورة </t>
         </is>
       </c>
     </row>
@@ -582,31 +582,31 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">لبنان </t>
+          <t xml:space="preserve">الاحتلال الإسرائيلي لجنوب لبنان </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">لبنان ,علم (راية) </t>
+          <t>-</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">بلد </t>
+          <t>-</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">قضاء المتن </t>
+          <t xml:space="preserve">جنوب لبنان </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>الاستخبارات والمراقبة والرصد (مترجمه)</t>
+          <t xml:space="preserve">لبنان </t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -616,58 +616,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">نهاريا </t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">لبنان ,علم (راية) </t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">بلد </t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>محصول (مترجمه)</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">الولايات المتحدة </t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">لبنان ,علم (راية) </t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">بلد </t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">زحلة </t>
+          <t xml:space="preserve">بيروت </t>
         </is>
       </c>
     </row>

</xml_diff>